<commit_message>
Fixed asset delta matrix to right shape. Modified accordingly load_asset_deltas and asset_scenarios. Removed asset names from asset_scenarios input arguments.
</commit_message>
<xml_diff>
--- a/entropy_pooling/sample_portfolio1_deltas.xlsx
+++ b/entropy_pooling/sample_portfolio1_deltas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ilmari/Documents/OR semma/entropy-poolin/entropy_pooling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60229ABC-1D17-E948-9D03-66483CF619AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADAFB3DA-2D85-7245-9834-924A2FE4E6CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1580" yWindow="2000" windowWidth="26840" windowHeight="14400" xr2:uid="{D749E855-D7F7-FB40-A8F6-2BBA7F3A4511}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>EUR Government Bonds</t>
   </si>
@@ -107,6 +107,45 @@
   </si>
   <si>
     <t>50Y EUR SWAP</t>
+  </si>
+  <si>
+    <t>EURUSD</t>
+  </si>
+  <si>
+    <t>US 10-Year Treasury Yield</t>
+  </si>
+  <si>
+    <t>Germany 10-Year Government Bond Yield</t>
+  </si>
+  <si>
+    <t>iVol US Equities</t>
+  </si>
+  <si>
+    <t>iVol European Equities</t>
+  </si>
+  <si>
+    <t>FED Balance Sheet Total</t>
+  </si>
+  <si>
+    <t>Eurosystem Balance Sheet Total</t>
+  </si>
+  <si>
+    <t>US Core Inflation</t>
+  </si>
+  <si>
+    <t>US Unemployment</t>
+  </si>
+  <si>
+    <t>US Manufacturing PMI</t>
+  </si>
+  <si>
+    <t>US Services PMI</t>
+  </si>
+  <si>
+    <t>Eurozone Core Inflation</t>
+  </si>
+  <si>
+    <t>Eurozone Unemployment</t>
   </si>
 </sst>
 </file>
@@ -458,304 +497,526 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5013DA17-9526-D14E-9C1D-CC2B329D2A6C}">
-  <dimension ref="A1:X4"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="K1" t="s">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>-1</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>-1</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>2</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-      <c r="V3">
-        <v>0</v>
-      </c>
-      <c r="W3">
-        <v>0</v>
-      </c>
-      <c r="X3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="X4">
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
         <v>0</v>
       </c>
     </row>

</xml_diff>